<commit_message>
remove police id excel importer
</commit_message>
<xml_diff>
--- a/public/excel/test.xlsx
+++ b/public/excel/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8.0.19\htdocs\mar\public\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hetlar\Desktop\spear\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F59EB95-ADC2-4994-85C9-119C169FB6E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81F1E74-9893-49EE-AD7B-9E2259E44B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2175" windowWidth="24240" windowHeight="13290" xr2:uid="{CF47734B-F3D3-47BE-9A83-319388EFF964}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23520" windowHeight="11775" xr2:uid="{CF47734B-F3D3-47BE-9A83-319388EFF964}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>رقم البوليصه</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>التاريخ</t>
   </si>
@@ -438,31 +435,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E78A980B-99BC-4AA4-99FB-5156BE964497}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="5" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" customWidth="1"/>
-    <col min="16" max="16" width="11.42578125" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="4" width="14" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
@@ -471,10 +467,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -483,10 +479,10 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -506,30 +502,27 @@
       <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="I8" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>